<commit_message>
Committing First Draft before making single-page changes Feb 29th 2020
</commit_message>
<xml_diff>
--- a/xml_to_csv/static/Login_creds.xlsx
+++ b/xml_to_csv/static/Login_creds.xlsx
@@ -416,7 +416,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2020-02-28 18:24:22.24S</t>
+          <t>2020-02-28 20:11:30.11S</t>
         </is>
       </c>
     </row>
@@ -443,7 +443,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2020-02-28 18:13:19.13S</t>
+          <t>2020-02-28 19:54:47.54S</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Second Draft with session-level error handling Mar 3rd 2020
</commit_message>
<xml_diff>
--- a/xml_to_csv/static/Login_creds.xlsx
+++ b/xml_to_csv/static/Login_creds.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -392,6 +392,11 @@
           <t>lastlogin</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>userid</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -416,8 +421,11 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2020-02-28 20:11:30.11S</t>
-        </is>
+          <t>2020-03-02 19:57:05.57S</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -443,8 +451,11 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2020-02-28 19:54:47.54S</t>
-        </is>
+          <t>2020-03-02 17:53:19.53S</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creating the first demo-ready version of the application
</commit_message>
<xml_diff>
--- a/xml_to_csv/static/Login_creds.xlsx
+++ b/xml_to_csv/static/Login_creds.xlsx
@@ -421,7 +421,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2020-03-02 19:57:05.57S</t>
+          <t>2020-03-12 18:13:26.13S</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -451,7 +451,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2020-03-02 17:53:19.53S</t>
+          <t>2020-03-11 21:48:46.48S</t>
         </is>
       </c>
       <c r="F3" t="n">

</xml_diff>

<commit_message>
Added notes and setup guide 13th Feb 2021
</commit_message>
<xml_diff>
--- a/xml_to_csv/static/Login_creds.xlsx
+++ b/xml_to_csv/static/Login_creds.xlsx
@@ -421,7 +421,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2020-03-12 18:13:26.13S</t>
+          <t>2020-03-15 20:25:47.25S</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -451,7 +451,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2020-03-11 21:48:46.48S</t>
+          <t>2020-03-22 20:03:37.03S</t>
         </is>
       </c>
       <c r="F3" t="n">

</xml_diff>

<commit_message>
Cleaning up codebase for containerization and deployment to Heroku
</commit_message>
<xml_diff>
--- a/xml_to_csv/static/Login_creds.xlsx
+++ b/xml_to_csv/static/Login_creds.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,7 +421,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2022-01-09 22:40:39.40S</t>
+          <t>2022-01-10 00:13:10.13S</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -456,6 +456,36 @@
       </c>
       <c r="F3" t="n">
         <v>101</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>vikrant</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Vikrant</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Deshpande</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>vikrant</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2022-01-10 00:12:59.12S</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated some random data
</commit_message>
<xml_diff>
--- a/xml_to_csv/static/Login_creds.xlsx
+++ b/xml_to_csv/static/Login_creds.xlsx
@@ -50,7 +50,6 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -66,6 +65,74 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -421,7 +488,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2022-01-10 00:32:01.32S</t>
+          <t>2022-01-10 00:55:35.55S</t>
         </is>
       </c>
       <c r="F2" t="n">

</xml_diff>

<commit_message>
Updated repo for cleanliness
</commit_message>
<xml_diff>
--- a/xml_to_csv/static/Login_creds.xlsx
+++ b/xml_to_csv/static/Login_creds.xlsx
@@ -50,7 +50,6 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -66,6 +65,74 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -481,7 +548,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2022-01-10 00:36:18.36S</t>
+          <t>2022-01-10 15:38:37.38S</t>
         </is>
       </c>
       <c r="F4" t="n">

</xml_diff>